<commit_message>
create result csv file
</commit_message>
<xml_diff>
--- a/모델링 결과.xlsx
+++ b/모델링 결과.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chank\Study\제주 관광객 소비패턴 변화 분석(BC카드)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AEFA6C-3959-498B-8216-55FCAC963BB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3667DD-30A3-47EC-81D3-B07818E10566}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F7FABCA6-915E-4274-904B-BB00832EB1E4}"/>
+    <workbookView xWindow="22824" yWindow="0" windowWidth="23256" windowHeight="12480" activeTab="1" xr2:uid="{F7FABCA6-915E-4274-904B-BB00832EB1E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Encoder에 따른 결과" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Ridge</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -275,6 +275,30 @@
   </si>
   <si>
     <t>Algorithm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LightGBM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num_boost_rounds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>min_child_weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max_depth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub_sample</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -285,7 +309,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +352,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -337,7 +369,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -481,13 +513,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -503,9 +557,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,18 +593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -569,13 +608,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -910,119 +970,119 @@
   <sheetData>
     <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>1.28</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <v>1.35</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>0.51</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="15">
         <v>0.41</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="15">
         <v>0.39</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <v>0.39</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>0.98</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>1.35</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>0.52</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>0.41</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="16">
         <v>0.39</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="16">
         <v>0.39</v>
       </c>
       <c r="I7" s="1"/>
@@ -1042,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72462259-4ECE-450C-9BE8-27305BA5BB5C}">
-  <dimension ref="B1:L17"/>
+  <dimension ref="B2:L36"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1053,7 +1113,8 @@
     <col min="1" max="1" width="1.625" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.125" bestFit="1" customWidth="1"/>
@@ -1061,546 +1122,1036 @@
     <col min="11" max="11" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="24.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:12" s="28" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+    </row>
+    <row r="3" spans="2:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="4" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L3" s="26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5" t="s">
+    <row r="4" spans="2:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11">
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10">
         <v>0.38450000000000001</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D5" s="10">
         <v>0.45700000000000002</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E5" s="9">
         <v>100</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F5" s="9">
         <v>0.3</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="10">
-        <v>1</v>
-      </c>
-      <c r="J4" s="10">
-        <v>1</v>
-      </c>
-      <c r="K4" s="10">
-        <f>IF(D4-C4=0,1,D4-C4)</f>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9">
+        <v>1</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" ref="K5:K16" si="0">IF(D5-C5=0,1,D5-C5)</f>
         <v>7.2500000000000009E-2</v>
       </c>
-      <c r="L4" s="10">
-        <f>RANK(K4,K$4:K$15,1)</f>
+      <c r="L5" s="9">
+        <f t="shared" ref="L5:L16" si="1">RANK(K5,K$5:K$16,1)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="7">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C6" s="11">
         <v>0.38429999999999997</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D6" s="11">
         <v>0.45579999999999998</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E6" s="6">
         <v>140</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F6" s="6">
         <v>0.25</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G6" s="6">
         <v>40</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H6" s="6">
         <v>10</v>
       </c>
-      <c r="I5" s="7">
-        <v>1</v>
-      </c>
-      <c r="J5" s="7">
-        <v>1</v>
-      </c>
-      <c r="K5" s="7">
-        <f>IF(D5-C5=0,1,D5-C5)</f>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
+        <f t="shared" si="0"/>
         <v>7.1500000000000008E-2</v>
       </c>
-      <c r="L5" s="7">
-        <f>RANK(K5,K$4:K$15,1)</f>
+      <c r="L6" s="6">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="7">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C7" s="11">
         <v>0.38369999999999999</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D7" s="11">
         <v>0.45650000000000002</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E7" s="6">
         <v>160</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F7" s="6">
         <v>0.25</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G7" s="6">
         <v>40</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H7" s="6">
         <v>10</v>
       </c>
-      <c r="I6" s="7">
-        <v>1</v>
-      </c>
-      <c r="J6" s="7">
-        <v>1</v>
-      </c>
-      <c r="K6" s="7">
-        <f>IF(D6-C6=0,1,D6-C6)</f>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="0"/>
         <v>7.2800000000000031E-2</v>
       </c>
-      <c r="L6" s="7">
-        <f>RANK(K6,K$4:K$15,1)</f>
+      <c r="L7" s="6">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="7">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C8" s="11">
         <v>0.38379999999999997</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D8" s="11">
         <v>0.45610000000000001</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E8" s="6">
         <v>150</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F8" s="6">
         <v>0.25</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G8" s="6">
         <v>40</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H8" s="6">
         <v>10</v>
       </c>
-      <c r="I7" s="7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="7">
-        <v>1</v>
-      </c>
-      <c r="K7" s="7">
-        <f>IF(D7-C7=0,1,D7-C7)</f>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="0"/>
         <v>7.2300000000000031E-2</v>
       </c>
-      <c r="L7" s="7">
-        <f>RANK(K7,K$4:K$15,1)</f>
+      <c r="L8" s="6">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="7">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C9" s="11">
         <v>0.38569999999999999</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D9" s="11">
         <v>0.45639999999999997</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E9" s="6">
         <v>140</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F9" s="6">
         <v>0.25</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G9" s="6">
         <v>40</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H9" s="6">
         <v>15</v>
       </c>
-      <c r="I8" s="7">
-        <v>1</v>
-      </c>
-      <c r="J8" s="7">
-        <v>1</v>
-      </c>
-      <c r="K8" s="7">
-        <f>IF(D8-C8=0,1,D8-C8)</f>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="0"/>
         <v>7.0699999999999985E-2</v>
       </c>
-      <c r="L8" s="7">
-        <f>RANK(K8,K$4:K$15,1)</f>
+      <c r="L9" s="6">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="7">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C10" s="11">
         <v>0.38900000000000001</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D10" s="11">
         <v>0.45639999999999997</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E10" s="6">
         <v>140</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="6">
         <v>0.25</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G10" s="6">
         <v>30</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H10" s="6">
         <v>10</v>
       </c>
-      <c r="I9" s="7">
-        <v>1</v>
-      </c>
-      <c r="J9" s="7">
-        <v>1</v>
-      </c>
-      <c r="K9" s="7">
-        <f>IF(D9-C9=0,1,D9-C9)</f>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="0"/>
         <v>6.739999999999996E-2</v>
       </c>
-      <c r="L9" s="7">
-        <f>RANK(K9,K$4:K$15,1)</f>
+      <c r="L10" s="6">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="7">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="6">
         <v>7</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C11" s="11">
         <v>0.38969999999999999</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D11" s="11">
         <v>0.45190000000000002</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E11" s="6">
         <v>140</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F11" s="6">
         <v>0.3</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G11" s="6">
         <v>30</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H11" s="6">
         <v>10</v>
       </c>
-      <c r="I10" s="7">
-        <v>1</v>
-      </c>
-      <c r="J10" s="7">
-        <v>1</v>
-      </c>
-      <c r="K10" s="7">
-        <f>IF(D10-C10=0,1,D10-C10)</f>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="0"/>
         <v>6.2200000000000033E-2</v>
       </c>
-      <c r="L10" s="7">
-        <f>RANK(K10,K$4:K$15,1)</f>
+      <c r="L11" s="6">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="7">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="6">
         <v>8</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C12" s="11">
         <v>0.38679999999999998</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D12" s="11">
         <v>0.46050000000000002</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E12" s="6">
         <v>130</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F12" s="6">
         <v>0.2</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G12" s="6">
         <v>40</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H12" s="6">
         <v>10</v>
       </c>
-      <c r="I11" s="7">
-        <v>1</v>
-      </c>
-      <c r="J11" s="7">
-        <v>1</v>
-      </c>
-      <c r="K11" s="7">
-        <f>IF(D11-C11=0,1,D11-C11)</f>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="0"/>
         <v>7.3700000000000043E-2</v>
       </c>
-      <c r="L11" s="7">
-        <f>RANK(K11,K$4:K$15,1)</f>
+      <c r="L12" s="6">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="7">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C13" s="11">
         <v>0.38719999999999999</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D13" s="11">
         <v>0.45829999999999999</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E13" s="6">
         <v>140</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F13" s="6">
         <v>0.3</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G13" s="6">
         <v>40</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H13" s="6">
         <v>10</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I13" s="6">
         <v>2</v>
       </c>
-      <c r="J12" s="7">
-        <v>1</v>
-      </c>
-      <c r="K12" s="7">
-        <f>IF(D12-C12=0,1,D12-C12)</f>
+      <c r="J13" s="6">
+        <v>1</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="0"/>
         <v>7.1099999999999997E-2</v>
       </c>
-      <c r="L12" s="7">
-        <f>RANK(K12,K$4:K$15,1)</f>
+      <c r="L13" s="6">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="7">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="6">
         <v>10</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C14" s="11">
         <v>0.38969999999999999</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D14" s="11">
         <v>0.45190000000000002</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E14" s="6">
         <v>140</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F14" s="6">
         <v>0.3</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G14" s="6">
         <v>30</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H14" s="6">
         <v>10</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I14" s="6">
         <v>2</v>
       </c>
-      <c r="J13" s="7">
-        <v>1</v>
-      </c>
-      <c r="K13" s="7">
-        <f>IF(D13-C13=0,1,D13-C13)</f>
+      <c r="J14" s="6">
+        <v>1</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="0"/>
         <v>6.2200000000000033E-2</v>
       </c>
-      <c r="L13" s="7">
-        <f>RANK(K13,K$4:K$15,1)</f>
+      <c r="L14" s="6">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="7">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="6">
         <v>11</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C15" s="11">
         <v>0.4037</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D15" s="11">
         <v>0.45450000000000002</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E15" s="6">
         <v>140</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F15" s="6">
         <v>0.3</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G15" s="6">
         <v>30</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H15" s="6">
         <v>10</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I15" s="6">
         <v>2</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J15" s="6">
         <v>0.5</v>
       </c>
-      <c r="K14" s="7">
-        <f>IF(D14-C14=0,1,D14-C14)</f>
+      <c r="K15" s="6">
+        <f t="shared" si="0"/>
         <v>5.0800000000000012E-2</v>
       </c>
-      <c r="L14" s="7">
-        <f>RANK(K14,K$4:K$15,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="8">
+      <c r="L15" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="7">
         <v>12</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C16" s="12">
         <v>0.4037</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D16" s="12">
         <v>0.45450000000000002</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E16" s="7">
         <v>140</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F16" s="7">
         <v>0.3</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G16" s="7">
         <v>30</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H16" s="7">
         <v>10</v>
       </c>
-      <c r="I15" s="8">
-        <v>1</v>
-      </c>
-      <c r="J15" s="8">
+      <c r="I16" s="7">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7">
         <v>0.5</v>
       </c>
-      <c r="K15" s="8">
-        <f>IF(D15-C15=0,1,D15-C15)</f>
+      <c r="K16" s="7">
+        <f t="shared" si="0"/>
         <v>5.0800000000000012E-2</v>
       </c>
-      <c r="L15" s="8">
-        <f>RANK(K15,K$4:K$15,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="3">
-        <f>MIN(C4:C15)</f>
-        <v>0.38369999999999999</v>
-      </c>
-      <c r="D16" s="3">
-        <f>MIN(D4:D15)</f>
-        <v>0.45190000000000002</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="L16" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3">
-        <f>MAX(C4:C15)</f>
-        <v>0.4037</v>
+        <f>MIN(C5:C16)</f>
+        <v>0.38369999999999999</v>
       </c>
       <c r="D17" s="3">
-        <f>MAX(D4:D15)</f>
-        <v>0.46050000000000002</v>
+        <f>MIN(D5:D16)</f>
+        <v>0.45190000000000002</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="L17" s="1"/>
     </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="3">
+        <f>MAX(C5:C16)</f>
+        <v>0.4037</v>
+      </c>
+      <c r="D18" s="3">
+        <f>MAX(D5:D16)</f>
+        <v>0.46050000000000002</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="20" spans="2:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+    </row>
+    <row r="21" spans="2:12" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="26"/>
+    </row>
+    <row r="23" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0.38879999999999998</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.46650000000000003</v>
+      </c>
+      <c r="E23" s="9">
+        <v>130</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="9">
+        <v>6</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9">
+        <f t="shared" ref="K23:K34" si="2">IF(D23-C23=0,1,D23-C23)</f>
+        <v>7.7700000000000047E-2</v>
+      </c>
+      <c r="L23" s="9">
+        <f>RANK(K23,K$23:K$34,1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="6">
+        <v>2</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.38879999999999998</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0.46650000000000003</v>
+      </c>
+      <c r="E24" s="6">
+        <v>140</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="9">
+        <v>6</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6">
+        <f t="shared" si="2"/>
+        <v>7.7700000000000047E-2</v>
+      </c>
+      <c r="L24" s="9">
+        <f t="shared" ref="L24:L34" si="3">RANK(K24,K$23:K$34,1)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="6">
+        <v>3</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="D25" s="11">
+        <v>0.46889999999999998</v>
+      </c>
+      <c r="E25" s="6">
+        <v>160</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="9">
+        <v>6</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6">
+        <f t="shared" si="2"/>
+        <v>7.6899999999999968E-2</v>
+      </c>
+      <c r="L25" s="9">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="6">
+        <v>4</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="D26" s="11">
+        <v>0.45710000000000001</v>
+      </c>
+      <c r="E26" s="6">
+        <v>200</v>
+      </c>
+      <c r="F26" s="6">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6">
+        <v>4</v>
+      </c>
+      <c r="H26" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="I26" s="6">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6">
+        <f t="shared" si="2"/>
+        <v>6.9599999999999995E-2</v>
+      </c>
+      <c r="L26" s="9">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="6">
+        <v>5</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0.3866</v>
+      </c>
+      <c r="D27" s="11">
+        <v>0.45739999999999997</v>
+      </c>
+      <c r="E27" s="6">
+        <v>160</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <v>4</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I27" s="6">
+        <v>1</v>
+      </c>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6">
+        <f t="shared" si="2"/>
+        <v>7.0799999999999974E-2</v>
+      </c>
+      <c r="L27" s="9">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="6">
+        <v>6</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="E28" s="6">
+        <v>160</v>
+      </c>
+      <c r="F28" s="6">
+        <v>1</v>
+      </c>
+      <c r="G28" s="6">
+        <v>4</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I28" s="6">
+        <v>1</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6">
+        <f t="shared" si="2"/>
+        <v>6.7900000000000016E-2</v>
+      </c>
+      <c r="L28" s="9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="6">
+        <v>7</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0.38440000000000002</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="E29" s="6">
+        <v>160</v>
+      </c>
+      <c r="F29" s="6">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6">
+        <v>6</v>
+      </c>
+      <c r="H29" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="6">
+        <v>1</v>
+      </c>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6">
+        <f t="shared" si="2"/>
+        <v>7.8600000000000003E-2</v>
+      </c>
+      <c r="L29" s="9">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="6">
+        <v>8</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0.40550000000000003</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0.46760000000000002</v>
+      </c>
+      <c r="E30" s="6">
+        <v>160</v>
+      </c>
+      <c r="F30" s="6">
+        <v>1</v>
+      </c>
+      <c r="G30" s="6">
+        <v>3</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="I30" s="6">
+        <v>1</v>
+      </c>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6">
+        <f t="shared" si="2"/>
+        <v>6.2099999999999989E-2</v>
+      </c>
+      <c r="L30" s="9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="6">
+        <v>9</v>
+      </c>
+      <c r="C31" s="11">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="E31" s="6">
+        <v>160</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="6">
+        <v>4</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I31" s="6">
+        <v>1</v>
+      </c>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6">
+        <f t="shared" si="2"/>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="L31" s="9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="6">
+        <v>10</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L32" s="9">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="6">
+        <v>11</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L33" s="9">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="7">
+        <v>12</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L34" s="9">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="3">
+        <f>MIN(C23:C34)</f>
+        <v>0.38440000000000002</v>
+      </c>
+      <c r="D35" s="3">
+        <f>MIN(D23:D34)</f>
+        <v>0.45590000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="3">
+        <f>MAX(C23:C34)</f>
+        <v>0.40550000000000003</v>
+      </c>
+      <c r="D36" s="3">
+        <f>MAX(D23:D34)</f>
+        <v>0.46889999999999998</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="E2:J2"/>
+  <mergeCells count="14">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="E3:J3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1608,7 +2159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35BEAD6-ACD6-40EF-824F-299D3AED8C8A}">
   <dimension ref="B1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1620,247 +2171,247 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" s="26" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="2:14" s="21" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>0</v>
       </c>
-      <c r="D2" s="9">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9">
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
         <v>2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>3</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>4</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>5</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>6</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="8">
         <v>7</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="8">
         <v>8</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="8">
         <v>9</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="8">
         <v>10</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="20">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="15"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
     </row>
     <row r="6" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
     </row>
     <row r="7" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
     </row>
     <row r="8" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>2014</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>2015</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>2016</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
     </row>
     <row r="9" spans="2:14" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="8">
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
         <v>10</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>11</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>12</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>2</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>3</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>4</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="7">
         <v>5</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="7">
         <v>6</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="7">
         <v>7</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="7">
         <v>8</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <v>9</v>
       </c>
     </row>

</xml_diff>